<commit_message>
Aggiornate chiamate con token con vendor corretto
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#ZUCCHETTIHEALTHCAREXX/Zucchetti_Healthcare/CSS2/2024_10/report-checklist.xlsx
+++ b/GATEWAY/A1#111#ZUCCHETTIHEALTHCAREXX/Zucchetti_Healthcare/CSS2/2024_10/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zucchettihealthcare.sharepoint.com/sites/Integrazioni/Shared Documents/General/FSE/Accreditamento/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uno\Git\it-fse-accreditamento-fork\GATEWAY\A1#111#ZUCCHETTIHEALTHCAREXX\Zucchetti_Healthcare\CSS2\2024_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{74014161-2822-4E87-A21B-E27B30B9F2BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DF48411-18F4-4129-B316-B840555B6BD4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168415C0-49EE-42D8-A7BE-19828DEAAF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4105,19 +4105,19 @@
     <t>09/05/2024  09:48:54.933</t>
   </si>
   <si>
-    <t>0b4468faefdf01f8</t>
-  </si>
-  <si>
-    <t>2024-05-14T12:01:18Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.3.1.4.4.6b86b273ff34fce19d6b804eff5a3f5747ada4eaa22f1d49c01e52ddb7875b4b.e4dc3bf276^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>3fe7c3437b397c89</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.3.1.4.4.6b86b273ff34fce19d6b804eff5a3f5747ada4eaa22f1d49c01e52ddb7875b4b.a915c9925a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-05-16T08:54:03Z</t>
+  </si>
+  <si>
+    <t>ae010e438e7bd9e6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.3.1.4.4.6b86b273ff34fce19d6b804eff5a3f5747ada4eaa22f1d49c01e52ddb7875b4b.8bd8083517^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f1da5abb9dd71584</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.3.1.4.4.6b86b273ff34fce19d6b804eff5a3f5747ada4eaa22f1d49c01e52ddb7875b4b.6beba200fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4464,6 +4464,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4478,9 +4481,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4565,10 +4565,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/namedSheetViews/namedSheetView1.xml><?xml version="1.0" encoding="utf-8"?>
-<namedSheetViews xmlns="http://schemas.microsoft.com/office/spreadsheetml/2019/namedsheetviews" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7075,10 +7071,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B384" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="I376" sqref="I376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7120,14 +7116,14 @@
       <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="38"/>
+      <c r="D2" s="39"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -7145,14 +7141,14 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="41"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -7170,12 +7166,12 @@
       <c r="T3" s="16"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="40" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="3"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -7194,12 +7190,12 @@
       <c r="T4" s="16"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="40" t="s">
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="40"/>
+      <c r="D5" s="41"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -7217,8 +7213,8 @@
       <c r="T5" s="16"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="1"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -7522,13 +7518,13 @@
         <v>63</v>
       </c>
       <c r="F15" s="23">
-        <v>45426</v>
-      </c>
-      <c r="G15" s="41" t="s">
+        <v>45428</v>
+      </c>
+      <c r="G15" s="36" t="s">
+        <v>860</v>
+      </c>
+      <c r="H15" s="24" t="s">
         <v>861</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>860</v>
       </c>
       <c r="I15" s="24" t="s">
         <v>862</v>
@@ -19934,10 +19930,10 @@
         <v>784</v>
       </c>
       <c r="F376" s="23">
-        <v>45426</v>
+        <v>45428</v>
       </c>
       <c r="G376" s="34" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="H376" s="24" t="s">
         <v>863</v>
@@ -27621,17 +27617,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e246371e-0fe6-4e60-9da6-0574cfff2d05">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d199676f-dea3-4248-b14d-078d8bf8a29a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046B2B26E4D726F47A11583A23F30D841" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="efecf3075541cf0ab36a77e730b75aaa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e246371e-0fe6-4e60-9da6-0574cfff2d05" xmlns:ns3="d199676f-dea3-4248-b14d-078d8bf8a29a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbb738678e67a851313bdd742041dd3b" ns2:_="" ns3:_="">
     <xsd:import namespace="e246371e-0fe6-4e60-9da6-0574cfff2d05"/>
@@ -27860,6 +27845,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e246371e-0fe6-4e60-9da6-0574cfff2d05">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d199676f-dea3-4248-b14d-078d8bf8a29a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -27870,6 +27866,25 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101055E-0134-4C55-B2BF-3C08EFA7B6A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e246371e-0fe6-4e60-9da6-0574cfff2d05"/>
+    <ds:schemaRef ds:uri="d199676f-dea3-4248-b14d-078d8bf8a29a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BC5383-9A39-44FE-820E-E8F909F971FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -27880,10 +27895,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101055E-0134-4C55-B2BF-3C08EFA7B6A6}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5435EEEA-4D16-432F-AD75-4FF12121BE2B}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Aggiornamento chiamate con token corretti
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#ZUCCHETTIHEALTHCAREXX/Zucchetti_Healthcare/CSS2/2024_10/report-checklist.xlsx
+++ b/GATEWAY/A1#111#ZUCCHETTIHEALTHCAREXX/Zucchetti_Healthcare/CSS2/2024_10/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uno\Git\it-fse-accreditamento-fork\GATEWAY\A1#111#ZUCCHETTIHEALTHCAREXX\Zucchetti_Healthcare\CSS2\2024_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168415C0-49EE-42D8-A7BE-19828DEAAF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C289932A-E853-4DB8-820A-AC98F1861B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4105,19 +4105,19 @@
     <t>09/05/2024  09:48:54.933</t>
   </si>
   <si>
-    <t>2024-05-16T08:54:03Z</t>
-  </si>
-  <si>
-    <t>ae010e438e7bd9e6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.3.1.4.4.6b86b273ff34fce19d6b804eff5a3f5747ada4eaa22f1d49c01e52ddb7875b4b.8bd8083517^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>f1da5abb9dd71584</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.3.1.4.4.6b86b273ff34fce19d6b804eff5a3f5747ada4eaa22f1d49c01e52ddb7875b4b.6beba200fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-05-17T09:02:23Z</t>
+  </si>
+  <si>
+    <t>149a685566425d7b</t>
+  </si>
+  <si>
+    <t>43736aef45a44463</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.3.1.4.4.6b86b273ff34fce19d6b804eff5a3f5747ada4eaa22f1d49c01e52ddb7875b4b.0039e816a1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.3.1.4.4.6b86b273ff34fce19d6b804eff5a3f5747ada4eaa22f1d49c01e52ddb7875b4b.5a3d01cfd3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -7071,7 +7071,7 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="I376" sqref="I376"/>
@@ -7518,7 +7518,7 @@
         <v>63</v>
       </c>
       <c r="F15" s="23">
-        <v>45428</v>
+        <v>45429</v>
       </c>
       <c r="G15" s="36" t="s">
         <v>860</v>
@@ -7527,7 +7527,7 @@
         <v>861</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>64</v>
@@ -19930,13 +19930,13 @@
         <v>784</v>
       </c>
       <c r="F376" s="23">
-        <v>45428</v>
+        <v>45429</v>
       </c>
       <c r="G376" s="34" t="s">
         <v>860</v>
       </c>
       <c r="H376" s="24" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="I376" s="24" t="s">
         <v>864</v>
@@ -27617,6 +27617,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e246371e-0fe6-4e60-9da6-0574cfff2d05">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d199676f-dea3-4248-b14d-078d8bf8a29a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046B2B26E4D726F47A11583A23F30D841" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="efecf3075541cf0ab36a77e730b75aaa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e246371e-0fe6-4e60-9da6-0574cfff2d05" xmlns:ns3="d199676f-dea3-4248-b14d-078d8bf8a29a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbb738678e67a851313bdd742041dd3b" ns2:_="" ns3:_="">
     <xsd:import namespace="e246371e-0fe6-4e60-9da6-0574cfff2d05"/>
@@ -27845,17 +27856,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e246371e-0fe6-4e60-9da6-0574cfff2d05">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d199676f-dea3-4248-b14d-078d8bf8a29a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -27866,6 +27866,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BC5383-9A39-44FE-820E-E8F909F971FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e246371e-0fe6-4e60-9da6-0574cfff2d05"/>
+    <ds:schemaRef ds:uri="d199676f-dea3-4248-b14d-078d8bf8a29a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101055E-0134-4C55-B2BF-3C08EFA7B6A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27884,17 +27895,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BC5383-9A39-44FE-820E-E8F909F971FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e246371e-0fe6-4e60-9da6-0574cfff2d05"/>
-    <ds:schemaRef ds:uri="d199676f-dea3-4248-b14d-078d8bf8a29a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5435EEEA-4D16-432F-AD75-4FF12121BE2B}">
   <ds:schemaRefs>

</xml_diff>